<commit_message>
authority list gets created from schedule
</commit_message>
<xml_diff>
--- a/CTC/Schedules/Green Line/Schedule 1.xlsx
+++ b/CTC/Schedules/Green Line/Schedule 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Trains C\trains\CTC\Schedules\Green Line\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C872537-C120-4168-826D-11D21E571E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4246A0F0-0DC7-4305-A3A3-2C91981D27B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1C060F58-93B1-4832-B2FF-881A9457D027}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{1C060F58-93B1-4832-B2FF-881A9457D027}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -98,10 +98,10 @@
     <t>STATION; INGLEWOOD IN</t>
   </si>
   <si>
-    <t>STATION; OVERBOOK IN</t>
-  </si>
-  <si>
     <t>Time to dispatch</t>
+  </si>
+  <si>
+    <t>STATION; OVERBROOK IN</t>
   </si>
 </sst>
 </file>
@@ -142,8 +142,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -482,7 +482,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,15 +505,15 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="2">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1">
         <v>30</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>60</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>90</v>
       </c>
     </row>
@@ -719,25 +719,25 @@
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed for red line
</commit_message>
<xml_diff>
--- a/CTC/Schedules/Green Line/Schedule 1.xlsx
+++ b/CTC/Schedules/Green Line/Schedule 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Trains C\trains\CTC\Schedules\Green Line\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4246A0F0-0DC7-4305-A3A3-2C91981D27B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7746AEE-EFBE-459E-9895-2014DF7291B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{1C060F58-93B1-4832-B2FF-881A9457D027}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{1C060F58-93B1-4832-B2FF-881A9457D027}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="23">
   <si>
     <t>Train 0</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>STATION; OVERBROOK IN</t>
+  </si>
+  <si>
+    <t>STATION; GLENBURY IN</t>
   </si>
 </sst>
 </file>
@@ -142,7 +145,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -479,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF8DEE79-2019-4A95-AA6E-77A99001E3D6}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,144 +602,155 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="2" t="s">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="1" t="s">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>